<commit_message>
expense import and export is working
</commit_message>
<xml_diff>
--- a/public/sample/excel/expenses-sample.xlsx
+++ b/public/sample/excel/expenses-sample.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -20,15 +20,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t xml:space="preserve">name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">status</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t xml:space="preserve">expense_type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">store</t>
+  </si>
+  <si>
+    <t xml:space="preserve">employee_code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">amount</t>
+  </si>
+  <si>
+    <t xml:space="preserve">expense_date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">note</t>
   </si>
 </sst>
 </file>
@@ -43,6 +52,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -102,8 +112,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -230,23 +248,40 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="7.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="4.93"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>